<commit_message>
Add result numbers for some quick-and-dirty prototype code which builds the VML using a single string and insertAdjacentHTML, rather than building up elements via the DOM API. Gives ~20% speedup.
</commit_message>
<xml_diff>
--- a/buttons/Performance Results - Buttons.xlsx
+++ b/buttons/Performance Results - Buttons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="-80" windowWidth="23560" windowHeight="17380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2040" yWindow="-80" windowWidth="23560" windowHeight="17380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IE6" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="22">
   <si>
     <t>Total time - 5 runs (ms)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +104,10 @@
   </si>
   <si>
     <t>Average Time Per Run (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standalone buttons - w/PIE - prototype using insertAdjacentHTML - 9/9/10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,23 +448,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="571551752"/>
-        <c:axId val="571548392"/>
+        <c:axId val="577287544"/>
+        <c:axId val="577234792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="571551752"/>
+        <c:axId val="577287544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571548392"/>
+        <c:crossAx val="577234792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="571548392"/>
+        <c:axId val="577234792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +472,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571551752"/>
+        <c:crossAx val="577287544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -704,23 +708,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678152424"/>
-        <c:axId val="678155496"/>
+        <c:axId val="577651368"/>
+        <c:axId val="577654440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678152424"/>
+        <c:axId val="577651368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678155496"/>
+        <c:crossAx val="577654440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678155496"/>
+        <c:axId val="577654440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +732,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678152424"/>
+        <c:crossAx val="577651368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -964,23 +968,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="590047512"/>
-        <c:axId val="678181736"/>
+        <c:axId val="577719704"/>
+        <c:axId val="577722776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="590047512"/>
+        <c:axId val="577719704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678181736"/>
+        <c:crossAx val="577722776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678181736"/>
+        <c:axId val="577722776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +992,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="590047512"/>
+        <c:crossAx val="577719704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1224,23 +1228,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678046296"/>
-        <c:axId val="678049368"/>
+        <c:axId val="579867592"/>
+        <c:axId val="579870664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678046296"/>
+        <c:axId val="579867592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678049368"/>
+        <c:crossAx val="579870664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678049368"/>
+        <c:axId val="579870664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1252,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678046296"/>
+        <c:crossAx val="579867592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1282,7 +1286,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$B$29</c:f>
+              <c:f>'IE7'!$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1293,7 +1297,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$48:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1320,27 +1324,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$B$30:$B$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>108.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>157.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>212.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>271.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>333.6666666666666</c:v>
+              <c:f>'IE7'!$B$48:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>398.6666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>641.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>894.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1130.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1386.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1351,7 +1355,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$C$29</c:f>
+              <c:f>'IE7'!$C$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1362,7 +1366,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$48:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1389,27 +1393,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$C$30:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>105.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>191.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>241.0</c:v>
+              <c:f>'IE7'!$C$48:$C$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1420,7 +1424,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$D$29</c:f>
+              <c:f>'IE7'!$D$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1431,7 +1435,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$48:$A$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1458,49 +1462,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$D$30:$D$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>173.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>262.3333333333334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>342.6666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>463.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>574.6666666666667</c:v>
+              <c:f>'IE7'!$D$48:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>441.3333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>685.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>955.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1197.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1473.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678282104"/>
-        <c:axId val="678285176"/>
+        <c:axId val="579934408"/>
+        <c:axId val="579937480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678282104"/>
+        <c:axId val="579934408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678285176"/>
+        <c:crossAx val="579937480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678285176"/>
+        <c:axId val="579937480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +1512,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678282104"/>
+        <c:crossAx val="579934408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1542,7 +1546,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$B$47</c:f>
+              <c:f>'IE7'!$B$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1553,7 +1557,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$48:$A$53</c:f>
+              <c:f>'IE7'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1580,27 +1584,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$B$48:$B$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>398.6666666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>641.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>894.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1130.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1386.0</c:v>
+              <c:f>'IE7'!$B$72:$B$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1087.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2230.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3768.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5710.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7850.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1611,7 +1615,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$C$47</c:f>
+              <c:f>'IE7'!$C$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1622,7 +1626,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$48:$A$53</c:f>
+              <c:f>'IE7'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1649,27 +1653,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$C$48:$C$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42.66666666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44.33333333333334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60.66666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.0</c:v>
+              <c:f>'IE7'!$C$72:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>234.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>326.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,7 +1684,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$D$47</c:f>
+              <c:f>'IE7'!$D$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1691,7 +1695,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$48:$A$53</c:f>
+              <c:f>'IE7'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1718,49 +1722,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$D$48:$D$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>441.3333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>685.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>955.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1197.333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1473.0</c:v>
+              <c:f>'IE7'!$D$72:$D$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1238.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2464.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4008.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6036.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8170.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678315960"/>
-        <c:axId val="569912600"/>
+        <c:axId val="522465736"/>
+        <c:axId val="514690264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678315960"/>
+        <c:axId val="522465736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569912600"/>
+        <c:crossAx val="514690264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="569912600"/>
+        <c:axId val="514690264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +1772,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678315960"/>
+        <c:crossAx val="522465736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2004,23 +2008,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="677925768"/>
-        <c:axId val="677928840"/>
+        <c:axId val="579994600"/>
+        <c:axId val="579997672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677925768"/>
+        <c:axId val="579994600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677928840"/>
+        <c:crossAx val="579997672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677928840"/>
+        <c:axId val="579997672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2032,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677925768"/>
+        <c:crossAx val="579994600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2264,23 +2268,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="677839032"/>
-        <c:axId val="677842104"/>
+        <c:axId val="580030632"/>
+        <c:axId val="580033704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677839032"/>
+        <c:axId val="580030632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677842104"/>
+        <c:crossAx val="580033704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677842104"/>
+        <c:axId val="580033704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,7 +2292,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677839032"/>
+        <c:crossAx val="580030632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2524,23 +2528,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678384088"/>
-        <c:axId val="678387160"/>
+        <c:axId val="580065080"/>
+        <c:axId val="580068152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678384088"/>
+        <c:axId val="580065080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678387160"/>
+        <c:crossAx val="580068152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678387160"/>
+        <c:axId val="580068152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,7 +2552,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678384088"/>
+        <c:crossAx val="580065080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2784,23 +2788,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678375176"/>
-        <c:axId val="677512616"/>
+        <c:axId val="580099704"/>
+        <c:axId val="580102776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678375176"/>
+        <c:axId val="580099704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677512616"/>
+        <c:crossAx val="580102776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677512616"/>
+        <c:axId val="580102776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,7 +2812,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678375176"/>
+        <c:crossAx val="580099704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3044,23 +3048,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678343752"/>
-        <c:axId val="678346824"/>
+        <c:axId val="580133992"/>
+        <c:axId val="580137064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678343752"/>
+        <c:axId val="580133992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678346824"/>
+        <c:crossAx val="580137064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678346824"/>
+        <c:axId val="580137064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,7 +3072,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678343752"/>
+        <c:crossAx val="580133992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3304,23 +3308,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="527493240"/>
-        <c:axId val="527656552"/>
+        <c:axId val="577237912"/>
+        <c:axId val="577236232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="527493240"/>
+        <c:axId val="577237912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527656552"/>
+        <c:crossAx val="577236232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="527656552"/>
+        <c:axId val="577236232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3328,7 +3332,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527493240"/>
+        <c:crossAx val="577237912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3564,23 +3568,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="677723224"/>
-        <c:axId val="677726296"/>
+        <c:axId val="580168472"/>
+        <c:axId val="580171544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677723224"/>
+        <c:axId val="580168472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677726296"/>
+        <c:crossAx val="580171544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677726296"/>
+        <c:axId val="580171544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3588,7 +3592,267 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677723224"/>
+        <c:crossAx val="580168472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'IE8'!$B$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'IE8'!$A$72:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'IE8'!$B$72:$B$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>787.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1524.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2628.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4029.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5201.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'IE8'!$C$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rendering time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'IE8'!$A$72:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'IE8'!$C$72:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'IE8'!$D$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total time - 5 runs (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'IE8'!$A$72:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'IE8'!$D$72:$D$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>796.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1538.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2651.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4065.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5236.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="584030872"/>
+        <c:axId val="584033944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="584030872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="584033944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="584033944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="584030872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3824,23 +4088,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="677901128"/>
-        <c:axId val="677904200"/>
+        <c:axId val="577425400"/>
+        <c:axId val="577428472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677901128"/>
+        <c:axId val="577425400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677904200"/>
+        <c:crossAx val="577428472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677904200"/>
+        <c:axId val="577428472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,7 +4112,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677901128"/>
+        <c:crossAx val="577425400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4084,23 +4348,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678101000"/>
-        <c:axId val="678104072"/>
+        <c:axId val="577460760"/>
+        <c:axId val="577463832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678101000"/>
+        <c:axId val="577460760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678104072"/>
+        <c:crossAx val="577463832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678104072"/>
+        <c:axId val="577463832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4108,7 +4372,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678101000"/>
+        <c:crossAx val="577460760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4344,23 +4608,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678242472"/>
-        <c:axId val="678238824"/>
+        <c:axId val="577494472"/>
+        <c:axId val="577497544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678242472"/>
+        <c:axId val="577494472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678238824"/>
+        <c:crossAx val="577497544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678238824"/>
+        <c:axId val="577497544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4368,7 +4632,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678242472"/>
+        <c:crossAx val="577494472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4604,23 +4868,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678207464"/>
-        <c:axId val="678261224"/>
+        <c:axId val="577528984"/>
+        <c:axId val="577532056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678207464"/>
+        <c:axId val="577528984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678261224"/>
+        <c:crossAx val="577532056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678261224"/>
+        <c:axId val="577532056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4628,7 +4892,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678207464"/>
+        <c:crossAx val="577528984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4662,7 +4926,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$B$2</c:f>
+              <c:f>'IE6'!$B$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4673,7 +4937,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$3:$A$8</c:f>
+              <c:f>'IE6'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4700,27 +4964,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$B$3:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>68.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>123.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>180.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>260.6666666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>309.6666666666666</c:v>
+              <c:f>'IE6'!$B$72:$B$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1113.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2325.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3718.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5430.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7333.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4731,7 +4995,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$C$2</c:f>
+              <c:f>'IE6'!$C$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4742,7 +5006,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$3:$A$8</c:f>
+              <c:f>'IE6'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4769,27 +5033,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$C$3:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81.66666666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>146.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>211.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>291.6666666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>370.3333333333333</c:v>
+              <c:f>'IE6'!$C$72:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>231.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4800,7 +5064,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$D$2</c:f>
+              <c:f>'IE6'!$D$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4811,7 +5075,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$3:$A$8</c:f>
+              <c:f>'IE6'!$A$72:$A$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4838,49 +5102,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$D$3:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>150.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>270.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>391.3333333333334</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>552.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>680.0</c:v>
+              <c:f>'IE6'!$D$72:$D$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1212.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2444.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3869.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5660.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7564.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="528296152"/>
-        <c:axId val="528299224"/>
+        <c:axId val="518948248"/>
+        <c:axId val="518829336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="528296152"/>
+        <c:axId val="518948248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="528299224"/>
+        <c:crossAx val="518829336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="528299224"/>
+        <c:axId val="518829336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4888,7 +5152,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="528296152"/>
+        <c:crossAx val="518948248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4922,7 +5186,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$B$11</c:f>
+              <c:f>'IE7'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4933,7 +5197,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$12:$A$17</c:f>
+              <c:f>'IE7'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4960,27 +5224,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$B$12:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1570.333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3269.666666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5533.333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8113.666666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11677.66666666667</c:v>
+              <c:f>'IE7'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260.6666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>309.6666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4991,7 +5255,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$C$11</c:f>
+              <c:f>'IE7'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5002,7 +5266,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$12:$A$17</c:f>
+              <c:f>'IE7'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5029,27 +5293,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$C$12:$C$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>186.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>202.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>242.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>241.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>345.0</c:v>
+              <c:f>'IE7'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>291.6666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>370.3333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5060,7 +5324,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$D$11</c:f>
+              <c:f>'IE7'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5071,7 +5335,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$12:$A$17</c:f>
+              <c:f>'IE7'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5098,49 +5362,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$D$12:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1756.333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3472.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5775.666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8354.666666666668</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12022.66666666667</c:v>
+              <c:f>'IE7'!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>270.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>391.3333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>552.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678106568"/>
-        <c:axId val="678109640"/>
+        <c:axId val="577581368"/>
+        <c:axId val="577584440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678106568"/>
+        <c:axId val="577581368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678109640"/>
+        <c:crossAx val="577584440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678109640"/>
+        <c:axId val="577584440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5148,7 +5412,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678106568"/>
+        <c:crossAx val="577581368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5182,7 +5446,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$B$29</c:f>
+              <c:f>'IE7'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5193,7 +5457,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$12:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5220,27 +5484,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$B$30:$B$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>108.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>157.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>212.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>271.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>333.6666666666666</c:v>
+              <c:f>'IE7'!$B$12:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1570.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3269.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5533.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8113.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11677.66666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5251,7 +5515,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$C$29</c:f>
+              <c:f>'IE7'!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5262,7 +5526,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$12:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5289,27 +5553,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$C$30:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.33333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>105.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>191.6666666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
+              <c:f>'IE7'!$C$12:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>186.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>345.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5320,7 +5584,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IE7'!$D$29</c:f>
+              <c:f>'IE7'!$D$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5331,7 +5595,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'IE7'!$A$30:$A$35</c:f>
+              <c:f>'IE7'!$A$12:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5358,49 +5622,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'IE7'!$D$30:$D$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>173.3333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>262.3333333333334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>342.6666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>463.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>574.6666666666667</c:v>
+              <c:f>'IE7'!$D$12:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1756.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3472.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5775.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8354.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12022.66666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="678190184"/>
-        <c:axId val="678197160"/>
+        <c:axId val="577616936"/>
+        <c:axId val="577620008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="678190184"/>
+        <c:axId val="577616936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678197160"/>
+        <c:crossAx val="577620008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678197160"/>
+        <c:axId val="577620008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5408,7 +5672,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="678190184"/>
+        <c:crossAx val="577616936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5609,6 +5873,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1739900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5707,36 +6001,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1536700</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>3073400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -5758,7 +6022,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5788,37 +6052,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1536700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>3073400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5848,7 +6082,37 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1803400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6034,6 +6298,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1422400</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6362,10 +6656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6434,7 +6728,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/5</f>
+        <f t="shared" ref="E3:E8" si="0">D3/5</f>
         <v>0</v>
       </c>
     </row>
@@ -6455,7 +6749,7 @@
         <v>126</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/5</f>
+        <f t="shared" si="0"/>
         <v>25.2</v>
       </c>
       <c r="F4">
@@ -6490,11 +6784,11 @@
         <v>87</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D8" si="0">SUM(B5:C5)</f>
+        <f t="shared" ref="D5:D8" si="1">SUM(B5:C5)</f>
         <v>224.33333333333334</v>
       </c>
       <c r="E5" s="5">
-        <f>D5/5</f>
+        <f t="shared" si="0"/>
         <v>44.866666666666667</v>
       </c>
       <c r="F5">
@@ -6529,11 +6823,11 @@
         <v>135.33333333333334</v>
       </c>
       <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>330.33333333333337</v>
+      </c>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>330.33333333333337</v>
-      </c>
-      <c r="E6" s="5">
-        <f>D6/5</f>
         <v>66.066666666666677</v>
       </c>
       <c r="F6">
@@ -6568,11 +6862,11 @@
         <v>157.33333333333334</v>
       </c>
       <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>414.33333333333337</v>
+      </c>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>414.33333333333337</v>
-      </c>
-      <c r="E7" s="5">
-        <f>D7/5</f>
         <v>82.866666666666674</v>
       </c>
       <c r="F7">
@@ -6607,11 +6901,11 @@
         <v>217.66666666666666</v>
       </c>
       <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>531.33333333333337</v>
+      </c>
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>531.33333333333337</v>
-      </c>
-      <c r="E8" s="5">
-        <f>D8/5</f>
         <v>106.26666666666668</v>
       </c>
       <c r="F8">
@@ -6694,7 +6988,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
-        <f>D12/5</f>
+        <f t="shared" ref="E12:E17" si="2">D12/5</f>
         <v>0</v>
       </c>
     </row>
@@ -6711,11 +7005,11 @@
         <v>80.333333333333329</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D17" si="1">SUM(B13:C13)</f>
+        <f t="shared" ref="D13:D17" si="3">SUM(B13:C13)</f>
         <v>1747.3333333333333</v>
       </c>
       <c r="E13" s="5">
-        <f>D13/5</f>
+        <f t="shared" si="2"/>
         <v>349.46666666666664</v>
       </c>
       <c r="F13">
@@ -6750,11 +7044,11 @@
         <v>109.33333333333333</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3724</v>
       </c>
       <c r="E14" s="5">
-        <f>D14/5</f>
+        <f t="shared" si="2"/>
         <v>744.8</v>
       </c>
       <c r="F14">
@@ -6789,11 +7083,11 @@
         <v>145</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6041</v>
       </c>
       <c r="E15" s="5">
-        <f>D15/5</f>
+        <f t="shared" si="2"/>
         <v>1208.2</v>
       </c>
       <c r="F15">
@@ -6828,11 +7122,11 @@
         <v>186</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9034.3333333333339</v>
       </c>
       <c r="E16" s="5">
-        <f>D16/5</f>
+        <f t="shared" si="2"/>
         <v>1806.8666666666668</v>
       </c>
       <c r="F16">
@@ -6867,11 +7161,11 @@
         <v>221.33333333333334</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11983.666666666668</v>
       </c>
       <c r="E17" s="5">
-        <f>D17/5</f>
+        <f t="shared" si="2"/>
         <v>2396.7333333333336</v>
       </c>
       <c r="F17">
@@ -6954,7 +7248,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5">
-        <f>D21/5</f>
+        <f t="shared" ref="E21:E26" si="4">D21/5</f>
         <v>0</v>
       </c>
     </row>
@@ -6971,11 +7265,11 @@
         <v>75</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:D26" si="2">SUM(B22:C22)</f>
+        <f t="shared" ref="D22:D26" si="5">SUM(B22:C22)</f>
         <v>1454</v>
       </c>
       <c r="E22" s="5">
-        <f>D22/5</f>
+        <f t="shared" si="4"/>
         <v>290.8</v>
       </c>
       <c r="F22">
@@ -7010,11 +7304,11 @@
         <v>115.33333333333333</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3068</v>
       </c>
       <c r="E23" s="5">
-        <f>D23/5</f>
+        <f t="shared" si="4"/>
         <v>613.6</v>
       </c>
       <c r="F23">
@@ -7049,11 +7343,11 @@
         <v>135</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4639.333333333333</v>
       </c>
       <c r="E24" s="5">
-        <f>D24/5</f>
+        <f t="shared" si="4"/>
         <v>927.86666666666656</v>
       </c>
       <c r="F24">
@@ -7088,11 +7382,11 @@
         <v>172</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6676.333333333333</v>
       </c>
       <c r="E25" s="5">
-        <f>D25/5</f>
+        <f t="shared" si="4"/>
         <v>1335.2666666666667</v>
       </c>
       <c r="F25">
@@ -7127,11 +7421,11 @@
         <v>195.66666666666666</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>8797.6666666666661</v>
       </c>
       <c r="E26" s="5">
-        <f>D26/5</f>
+        <f t="shared" si="4"/>
         <v>1759.5333333333333</v>
       </c>
       <c r="F26">
@@ -7208,11 +7502,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" ref="D30:D35" si="3">SUM(B30:C30)</f>
+        <f t="shared" ref="D30:D35" si="6">SUM(B30:C30)</f>
         <v>0</v>
       </c>
       <c r="E30" s="5">
-        <f>D30/5</f>
+        <f t="shared" ref="E30:E35" si="7">D30/5</f>
         <v>0</v>
       </c>
     </row>
@@ -7229,11 +7523,11 @@
         <v>47</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>226.66666666666666</v>
       </c>
       <c r="E31" s="5">
-        <f>D31/5</f>
+        <f t="shared" si="7"/>
         <v>45.333333333333329</v>
       </c>
       <c r="F31">
@@ -7268,11 +7562,11 @@
         <v>75.666666666666671</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>314</v>
       </c>
       <c r="E32" s="5">
-        <f>D32/5</f>
+        <f t="shared" si="7"/>
         <v>62.8</v>
       </c>
       <c r="F32">
@@ -7307,11 +7601,11 @@
         <v>95.333333333333329</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>373.33333333333331</v>
       </c>
       <c r="E33" s="5">
-        <f>D33/5</f>
+        <f t="shared" si="7"/>
         <v>74.666666666666657</v>
       </c>
       <c r="F33">
@@ -7346,11 +7640,11 @@
         <v>106.33333333333333</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>449</v>
       </c>
       <c r="E34" s="5">
-        <f>D34/5</f>
+        <f t="shared" si="7"/>
         <v>89.8</v>
       </c>
       <c r="F34">
@@ -7385,11 +7679,11 @@
         <v>128.33333333333334</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>573.66666666666663</v>
       </c>
       <c r="E35" s="5">
-        <f>D35/5</f>
+        <f t="shared" si="7"/>
         <v>114.73333333333332</v>
       </c>
       <c r="F35">
@@ -7468,11 +7762,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" ref="D39:D44" si="4">SUM(B39:C39)</f>
+        <f t="shared" ref="D39:D44" si="8">SUM(B39:C39)</f>
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <f>D39/5</f>
+        <f t="shared" ref="E39:E44" si="9">D39/5</f>
         <v>0</v>
       </c>
     </row>
@@ -7489,11 +7783,11 @@
         <v>26.666666666666668</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1043</v>
       </c>
       <c r="E40" s="5">
-        <f>D40/5</f>
+        <f t="shared" si="9"/>
         <v>208.6</v>
       </c>
       <c r="F40">
@@ -7528,11 +7822,11 @@
         <v>57</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2008.3333333333333</v>
       </c>
       <c r="E41" s="5">
-        <f>D41/5</f>
+        <f t="shared" si="9"/>
         <v>401.66666666666663</v>
       </c>
       <c r="F41">
@@ -7567,11 +7861,11 @@
         <v>51.333333333333336</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3026.666666666667</v>
       </c>
       <c r="E42" s="5">
-        <f>D42/5</f>
+        <f t="shared" si="9"/>
         <v>605.33333333333337</v>
       </c>
       <c r="F42">
@@ -7606,11 +7900,11 @@
         <v>52.666666666666664</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4233.3333333333339</v>
       </c>
       <c r="E43" s="5">
-        <f>D43/5</f>
+        <f t="shared" si="9"/>
         <v>846.66666666666674</v>
       </c>
       <c r="F43">
@@ -7645,11 +7939,11 @@
         <v>49.333333333333336</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5628</v>
       </c>
       <c r="E44" s="5">
-        <f>D44/5</f>
+        <f t="shared" si="9"/>
         <v>1125.5999999999999</v>
       </c>
       <c r="F44">
@@ -7728,11 +8022,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" ref="D48:D53" si="5">SUM(B48:C48)</f>
+        <f t="shared" ref="D48:D53" si="10">SUM(B48:C48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <f>D48/5</f>
+        <f t="shared" ref="E48:E53" si="11">D48/5</f>
         <v>0</v>
       </c>
     </row>
@@ -7749,11 +8043,11 @@
         <v>39.333333333333336</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>460.33333333333331</v>
       </c>
       <c r="E49" s="5">
-        <f>D49/5</f>
+        <f t="shared" si="11"/>
         <v>92.066666666666663</v>
       </c>
       <c r="F49">
@@ -7788,11 +8082,11 @@
         <v>34.333333333333336</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>671.66666666666674</v>
       </c>
       <c r="E50" s="5">
-        <f>D50/5</f>
+        <f t="shared" si="11"/>
         <v>134.33333333333334</v>
       </c>
       <c r="F50">
@@ -7827,11 +8121,11 @@
         <v>46.666666666666664</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>963</v>
       </c>
       <c r="E51" s="5">
-        <f>D51/5</f>
+        <f t="shared" si="11"/>
         <v>192.6</v>
       </c>
       <c r="F51">
@@ -7866,11 +8160,11 @@
         <v>50.666666666666664</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1195.6666666666667</v>
       </c>
       <c r="E52" s="5">
-        <f>D52/5</f>
+        <f t="shared" si="11"/>
         <v>239.13333333333335</v>
       </c>
       <c r="F52">
@@ -7905,11 +8199,11 @@
         <v>58.666666666666664</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1435.6666666666667</v>
       </c>
       <c r="E53" s="5">
-        <f>D53/5</f>
+        <f t="shared" si="11"/>
         <v>287.13333333333333</v>
       </c>
       <c r="F53">
@@ -7934,6 +8228,248 @@
     <row r="54" spans="1:11" s="2" customFormat="1" ht="150" customHeight="1">
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
+    </row>
+    <row r="70" spans="1:11" s="1" customFormat="1">
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" t="s">
+        <v>9</v>
+      </c>
+      <c r="K71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <f t="shared" ref="D72:D77" si="12">SUM(B72:C72)</f>
+        <v>0</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" ref="E72:E77" si="13">D72/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <f>AVERAGE(F73:H73)</f>
+        <v>1113.5</v>
+      </c>
+      <c r="C73">
+        <f>AVERAGE(I73:K73)</f>
+        <v>99</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="12"/>
+        <v>1212.5</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="13"/>
+        <v>242.5</v>
+      </c>
+      <c r="F73">
+        <v>1098</v>
+      </c>
+      <c r="G73">
+        <v>1129</v>
+      </c>
+      <c r="I73">
+        <v>101</v>
+      </c>
+      <c r="J73">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <f>AVERAGE(F74:H74)</f>
+        <v>2325</v>
+      </c>
+      <c r="C74">
+        <f>AVERAGE(I74:K74)</f>
+        <v>119</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="12"/>
+        <v>2444</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="13"/>
+        <v>488.8</v>
+      </c>
+      <c r="F74">
+        <v>2325</v>
+      </c>
+      <c r="G74">
+        <v>2325</v>
+      </c>
+      <c r="I74">
+        <v>124</v>
+      </c>
+      <c r="J74">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>60</v>
+      </c>
+      <c r="B75">
+        <f>AVERAGE(F75:H75)</f>
+        <v>3718</v>
+      </c>
+      <c r="C75">
+        <f>AVERAGE(I75:K75)</f>
+        <v>151</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="12"/>
+        <v>3869</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="13"/>
+        <v>773.8</v>
+      </c>
+      <c r="F75">
+        <v>3732</v>
+      </c>
+      <c r="G75">
+        <v>3700</v>
+      </c>
+      <c r="H75">
+        <v>3722</v>
+      </c>
+      <c r="I75">
+        <v>154</v>
+      </c>
+      <c r="J75">
+        <v>150</v>
+      </c>
+      <c r="K75">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <f>AVERAGE(F76:H76)</f>
+        <v>5430.5</v>
+      </c>
+      <c r="C76">
+        <f>AVERAGE(I76:K76)</f>
+        <v>230</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="12"/>
+        <v>5660.5</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="13"/>
+        <v>1132.0999999999999</v>
+      </c>
+      <c r="F76">
+        <v>5496</v>
+      </c>
+      <c r="G76">
+        <v>5365</v>
+      </c>
+      <c r="I76">
+        <v>250</v>
+      </c>
+      <c r="J76">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>100</v>
+      </c>
+      <c r="B77">
+        <f>AVERAGE(F77:H77)</f>
+        <v>7333</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(I77:K77)</f>
+        <v>231</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="12"/>
+        <v>7564</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="13"/>
+        <v>1512.8</v>
+      </c>
+      <c r="F77">
+        <v>7319</v>
+      </c>
+      <c r="G77">
+        <v>7244</v>
+      </c>
+      <c r="H77">
+        <v>7436</v>
+      </c>
+      <c r="I77">
+        <v>249</v>
+      </c>
+      <c r="J77">
+        <v>223</v>
+      </c>
+      <c r="K77">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="150" customHeight="1">
+      <c r="D78" s="4"/>
+      <c r="E78" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7950,10 +8486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8022,7 +8558,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/5</f>
+        <f t="shared" ref="E3:E8" si="0">D3/5</f>
         <v>0</v>
       </c>
     </row>
@@ -8043,7 +8579,7 @@
         <v>150</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/5</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F4">
@@ -8078,11 +8614,11 @@
         <v>146.66666666666666</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5" si="0">SUM(B5:C5)</f>
+        <f t="shared" ref="D5" si="1">SUM(B5:C5)</f>
         <v>270.33333333333331</v>
       </c>
       <c r="E5" s="5">
-        <f>D5/5</f>
+        <f t="shared" si="0"/>
         <v>54.066666666666663</v>
       </c>
       <c r="F5">
@@ -8117,11 +8653,11 @@
         <v>211.33333333333334</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D8" si="1">SUM(B6:C6)</f>
+        <f t="shared" ref="D6:D8" si="2">SUM(B6:C6)</f>
         <v>391.33333333333337</v>
       </c>
       <c r="E6" s="5">
-        <f>D6/5</f>
+        <f t="shared" si="0"/>
         <v>78.26666666666668</v>
       </c>
       <c r="F6">
@@ -8156,11 +8692,11 @@
         <v>291.66666666666669</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>552.33333333333337</v>
       </c>
       <c r="E7" s="5">
-        <f>D7/5</f>
+        <f t="shared" si="0"/>
         <v>110.46666666666667</v>
       </c>
       <c r="F7">
@@ -8195,11 +8731,11 @@
         <v>370.33333333333331</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>680</v>
       </c>
       <c r="E8" s="5">
-        <f>D8/5</f>
+        <f t="shared" si="0"/>
         <v>136</v>
       </c>
       <c r="F8">
@@ -8282,7 +8818,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
-        <f>D12/5</f>
+        <f t="shared" ref="E12:E17" si="3">D12/5</f>
         <v>0</v>
       </c>
     </row>
@@ -8299,11 +8835,11 @@
         <v>186</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D17" si="2">SUM(B13:C13)</f>
+        <f t="shared" ref="D13:D17" si="4">SUM(B13:C13)</f>
         <v>1756.3333333333333</v>
       </c>
       <c r="E13" s="5">
-        <f>D13/5</f>
+        <f t="shared" si="3"/>
         <v>351.26666666666665</v>
       </c>
       <c r="F13">
@@ -8338,11 +8874,11 @@
         <v>202.33333333333334</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" ref="D14" si="3">SUM(B14:C14)</f>
+        <f t="shared" ref="D14" si="5">SUM(B14:C14)</f>
         <v>3472</v>
       </c>
       <c r="E14" s="5">
-        <f>D14/5</f>
+        <f t="shared" si="3"/>
         <v>694.4</v>
       </c>
       <c r="F14">
@@ -8377,11 +8913,11 @@
         <v>242.33333333333334</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5775.6666666666661</v>
       </c>
       <c r="E15" s="5">
-        <f>D15/5</f>
+        <f t="shared" si="3"/>
         <v>1155.1333333333332</v>
       </c>
       <c r="F15">
@@ -8416,11 +8952,11 @@
         <v>241</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8354.6666666666679</v>
       </c>
       <c r="E16" s="5">
-        <f>D16/5</f>
+        <f t="shared" si="3"/>
         <v>1670.9333333333336</v>
       </c>
       <c r="F16">
@@ -8455,11 +8991,11 @@
         <v>345</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12022.666666666666</v>
       </c>
       <c r="E17" s="5">
-        <f>D17/5</f>
+        <f t="shared" si="3"/>
         <v>2404.5333333333333</v>
       </c>
       <c r="F17">
@@ -8542,7 +9078,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5">
-        <f>D21/5</f>
+        <f t="shared" ref="E21:E26" si="6">D21/5</f>
         <v>0</v>
       </c>
     </row>
@@ -8559,11 +9095,11 @@
         <v>123.66666666666667</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:D26" si="4">SUM(B22:C22)</f>
+        <f t="shared" ref="D22:D26" si="7">SUM(B22:C22)</f>
         <v>1415.3333333333335</v>
       </c>
       <c r="E22" s="5">
-        <f>D22/5</f>
+        <f t="shared" si="6"/>
         <v>283.06666666666672</v>
       </c>
       <c r="F22">
@@ -8598,11 +9134,11 @@
         <v>179.66666666666666</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2930</v>
       </c>
       <c r="E23" s="5">
-        <f>D23/5</f>
+        <f t="shared" si="6"/>
         <v>586</v>
       </c>
       <c r="F23">
@@ -8637,11 +9173,11 @@
         <v>218</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4695.666666666667</v>
       </c>
       <c r="E24" s="5">
-        <f>D24/5</f>
+        <f t="shared" si="6"/>
         <v>939.13333333333344</v>
       </c>
       <c r="F24">
@@ -8676,11 +9212,11 @@
         <v>296</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6859.333333333333</v>
       </c>
       <c r="E25" s="5">
-        <f>D25/5</f>
+        <f t="shared" si="6"/>
         <v>1371.8666666666666</v>
       </c>
       <c r="F25">
@@ -8715,11 +9251,11 @@
         <v>311.66666666666669</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9436</v>
       </c>
       <c r="E26" s="5">
-        <f>D26/5</f>
+        <f t="shared" si="6"/>
         <v>1887.2</v>
       </c>
       <c r="F26">
@@ -8797,11 +9333,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" ref="D30:D35" si="5">SUM(B30:C30)</f>
+        <f t="shared" ref="D30:D35" si="8">SUM(B30:C30)</f>
         <v>0</v>
       </c>
       <c r="E30" s="5">
-        <f>D30/5</f>
+        <f t="shared" ref="E30:E35" si="9">D30/5</f>
         <v>0</v>
       </c>
     </row>
@@ -8818,11 +9354,11 @@
         <v>65.333333333333329</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" ref="D31" si="6">SUM(B31:C31)</f>
+        <f t="shared" ref="D31" si="10">SUM(B31:C31)</f>
         <v>173.33333333333331</v>
       </c>
       <c r="E31" s="5">
-        <f>D31/5</f>
+        <f t="shared" si="9"/>
         <v>34.666666666666664</v>
       </c>
       <c r="F31">
@@ -8857,11 +9393,11 @@
         <v>105</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>262.33333333333337</v>
       </c>
       <c r="E32" s="5">
-        <f>D32/5</f>
+        <f t="shared" si="9"/>
         <v>52.466666666666676</v>
       </c>
       <c r="F32">
@@ -8896,11 +9432,11 @@
         <v>130.66666666666666</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>342.66666666666663</v>
       </c>
       <c r="E33" s="5">
-        <f>D33/5</f>
+        <f t="shared" si="9"/>
         <v>68.533333333333331</v>
       </c>
       <c r="F33">
@@ -8935,11 +9471,11 @@
         <v>191.66666666666666</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>463</v>
       </c>
       <c r="E34" s="5">
-        <f>D34/5</f>
+        <f t="shared" si="9"/>
         <v>92.6</v>
       </c>
       <c r="F34">
@@ -8974,11 +9510,11 @@
         <v>241</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>574.66666666666674</v>
       </c>
       <c r="E35" s="5">
-        <f>D35/5</f>
+        <f t="shared" si="9"/>
         <v>114.93333333333335</v>
       </c>
       <c r="F35">
@@ -9057,11 +9593,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" ref="D39:D44" si="7">SUM(B39:C39)</f>
+        <f t="shared" ref="D39:D44" si="11">SUM(B39:C39)</f>
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <f>D39/5</f>
+        <f t="shared" ref="E39:E44" si="12">D39/5</f>
         <v>0</v>
       </c>
     </row>
@@ -9078,11 +9614,11 @@
         <v>40.333333333333336</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" ref="D40" si="8">SUM(B40:C40)</f>
+        <f t="shared" ref="D40" si="13">SUM(B40:C40)</f>
         <v>873.33333333333337</v>
       </c>
       <c r="E40" s="5">
-        <f>D40/5</f>
+        <f t="shared" si="12"/>
         <v>174.66666666666669</v>
       </c>
       <c r="F40">
@@ -9117,11 +9653,11 @@
         <v>57.333333333333336</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1777</v>
       </c>
       <c r="E41" s="5">
-        <f>D41/5</f>
+        <f t="shared" si="12"/>
         <v>355.4</v>
       </c>
       <c r="F41">
@@ -9156,11 +9692,11 @@
         <v>61.666666666666664</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>2828</v>
       </c>
       <c r="E42" s="5">
-        <f>D42/5</f>
+        <f t="shared" si="12"/>
         <v>565.6</v>
       </c>
       <c r="F42">
@@ -9195,11 +9731,11 @@
         <v>74.333333333333329</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4085.666666666667</v>
       </c>
       <c r="E43" s="5">
-        <f>D43/5</f>
+        <f t="shared" si="12"/>
         <v>817.13333333333344</v>
       </c>
       <c r="F43">
@@ -9234,11 +9770,11 @@
         <v>76.666666666666671</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5612.666666666667</v>
       </c>
       <c r="E44" s="5">
-        <f>D44/5</f>
+        <f t="shared" si="12"/>
         <v>1122.5333333333333</v>
       </c>
       <c r="F44">
@@ -9317,11 +9853,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" ref="D48:D53" si="9">SUM(B48:C48)</f>
+        <f t="shared" ref="D48:D53" si="14">SUM(B48:C48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <f>D48/5</f>
+        <f t="shared" ref="E48:E53" si="15">D48/5</f>
         <v>0</v>
       </c>
     </row>
@@ -9338,11 +9874,11 @@
         <v>42.666666666666664</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>441.33333333333337</v>
       </c>
       <c r="E49" s="5">
-        <f>D49/5</f>
+        <f t="shared" si="15"/>
         <v>88.26666666666668</v>
       </c>
       <c r="F49">
@@ -9377,11 +9913,11 @@
         <v>44.333333333333336</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>685.66666666666674</v>
       </c>
       <c r="E50" s="5">
-        <f>D50/5</f>
+        <f t="shared" si="15"/>
         <v>137.13333333333335</v>
       </c>
       <c r="F50">
@@ -9416,11 +9952,11 @@
         <v>60.666666666666664</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>955</v>
       </c>
       <c r="E51" s="5">
-        <f>D51/5</f>
+        <f t="shared" si="15"/>
         <v>191</v>
       </c>
       <c r="F51">
@@ -9455,11 +9991,11 @@
         <v>67.333333333333329</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1197.3333333333333</v>
       </c>
       <c r="E52" s="5">
-        <f>D52/5</f>
+        <f t="shared" si="15"/>
         <v>239.46666666666664</v>
       </c>
       <c r="F52">
@@ -9494,11 +10030,11 @@
         <v>87</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1473</v>
       </c>
       <c r="E53" s="5">
-        <f>D53/5</f>
+        <f t="shared" si="15"/>
         <v>294.60000000000002</v>
       </c>
       <c r="F53">
@@ -9523,6 +10059,236 @@
     <row r="54" spans="1:11" s="2" customFormat="1" ht="152" customHeight="1">
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
+    </row>
+    <row r="70" spans="1:11" s="1" customFormat="1">
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" t="s">
+        <v>9</v>
+      </c>
+      <c r="K71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <f t="shared" ref="D72:D77" si="16">SUM(B72:C72)</f>
+        <v>0</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" ref="E72:E77" si="17">D72/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <f>AVERAGE(F73:H73)</f>
+        <v>1087.5</v>
+      </c>
+      <c r="C73">
+        <f>AVERAGE(I73:K73)</f>
+        <v>151</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="16"/>
+        <v>1238.5</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="17"/>
+        <v>247.7</v>
+      </c>
+      <c r="F73">
+        <v>1143</v>
+      </c>
+      <c r="G73">
+        <v>1032</v>
+      </c>
+      <c r="I73">
+        <v>132</v>
+      </c>
+      <c r="J73">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <f>AVERAGE(F74:H74)</f>
+        <v>2230.5</v>
+      </c>
+      <c r="C74">
+        <f>AVERAGE(I74:K74)</f>
+        <v>234</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="16"/>
+        <v>2464.5</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="17"/>
+        <v>492.9</v>
+      </c>
+      <c r="F74">
+        <v>2207</v>
+      </c>
+      <c r="G74">
+        <v>2254</v>
+      </c>
+      <c r="I74">
+        <v>237</v>
+      </c>
+      <c r="J74">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>60</v>
+      </c>
+      <c r="B75">
+        <f>AVERAGE(F75:H75)</f>
+        <v>3768</v>
+      </c>
+      <c r="C75">
+        <f>AVERAGE(I75:K75)</f>
+        <v>240.5</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="16"/>
+        <v>4008.5</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="17"/>
+        <v>801.7</v>
+      </c>
+      <c r="F75">
+        <v>3799</v>
+      </c>
+      <c r="G75">
+        <v>3737</v>
+      </c>
+      <c r="I75">
+        <v>273</v>
+      </c>
+      <c r="J75">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <f>AVERAGE(F76:H76)</f>
+        <v>5710.5</v>
+      </c>
+      <c r="C76">
+        <f>AVERAGE(I76:K76)</f>
+        <v>326</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="16"/>
+        <v>6036.5</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="17"/>
+        <v>1207.3</v>
+      </c>
+      <c r="F76">
+        <v>5739</v>
+      </c>
+      <c r="G76">
+        <v>5682</v>
+      </c>
+      <c r="I76">
+        <v>312</v>
+      </c>
+      <c r="J76">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>100</v>
+      </c>
+      <c r="B77">
+        <f>AVERAGE(F77:H77)</f>
+        <v>7850</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(I77:K77)</f>
+        <v>320.5</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="16"/>
+        <v>8170.5</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="17"/>
+        <v>1634.1</v>
+      </c>
+      <c r="F77">
+        <v>7779</v>
+      </c>
+      <c r="G77">
+        <v>7921</v>
+      </c>
+      <c r="I77">
+        <v>292</v>
+      </c>
+      <c r="J77">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="152" customHeight="1">
+      <c r="D78" s="4"/>
+      <c r="E78" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -9539,10 +10305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9611,7 +10377,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/5</f>
+        <f t="shared" ref="E3:E8" si="0">D3/5</f>
         <v>0</v>
       </c>
     </row>
@@ -9632,7 +10398,7 @@
         <v>224.66666666666666</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/5</f>
+        <f t="shared" si="0"/>
         <v>44.93333333333333</v>
       </c>
       <c r="F4">
@@ -9667,11 +10433,11 @@
         <v>336.66666666666669</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D8" si="0">SUM(B5:C5)</f>
+        <f t="shared" ref="D5:D8" si="1">SUM(B5:C5)</f>
         <v>425</v>
       </c>
       <c r="E5" s="5">
-        <f>D5/5</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="F5">
@@ -9706,11 +10472,11 @@
         <v>522.66666666666663</v>
       </c>
       <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>646</v>
+      </c>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>646</v>
-      </c>
-      <c r="E6" s="5">
-        <f>D6/5</f>
         <v>129.19999999999999</v>
       </c>
       <c r="F6">
@@ -9745,11 +10511,11 @@
         <v>654.66666666666663</v>
       </c>
       <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>817.66666666666663</v>
+      </c>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>817.66666666666663</v>
-      </c>
-      <c r="E7" s="5">
-        <f>D7/5</f>
         <v>163.53333333333333</v>
       </c>
       <c r="F7">
@@ -9784,11 +10550,11 @@
         <v>843.33333333333337</v>
       </c>
       <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>1073.3333333333335</v>
+      </c>
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>1073.3333333333335</v>
-      </c>
-      <c r="E8" s="5">
-        <f>D8/5</f>
         <v>214.66666666666669</v>
       </c>
       <c r="F8">
@@ -9871,7 +10637,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
-        <f>D12/5</f>
+        <f t="shared" ref="E12:E17" si="2">D12/5</f>
         <v>0</v>
       </c>
     </row>
@@ -9888,11 +10654,11 @@
         <v>10</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D17" si="1">SUM(B13:C13)</f>
+        <f t="shared" ref="D13:D17" si="3">SUM(B13:C13)</f>
         <v>1004.6666666666666</v>
       </c>
       <c r="E13" s="5">
-        <f>D13/5</f>
+        <f t="shared" si="2"/>
         <v>200.93333333333334</v>
       </c>
       <c r="F13">
@@ -9927,11 +10693,11 @@
         <v>17</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2285.3333333333335</v>
       </c>
       <c r="E14" s="5">
-        <f>D14/5</f>
+        <f t="shared" si="2"/>
         <v>457.06666666666672</v>
       </c>
       <c r="F14">
@@ -9966,11 +10732,11 @@
         <v>27.333333333333332</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3957.3333333333335</v>
       </c>
       <c r="E15" s="5">
-        <f>D15/5</f>
+        <f t="shared" si="2"/>
         <v>791.4666666666667</v>
       </c>
       <c r="F15">
@@ -10005,11 +10771,11 @@
         <v>36</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6164.333333333333</v>
       </c>
       <c r="E16" s="5">
-        <f>D16/5</f>
+        <f t="shared" si="2"/>
         <v>1232.8666666666666</v>
       </c>
       <c r="F16">
@@ -10044,11 +10810,11 @@
         <v>39.666666666666664</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8793.3333333333321</v>
       </c>
       <c r="E17" s="5">
-        <f>D17/5</f>
+        <f t="shared" si="2"/>
         <v>1758.6666666666665</v>
       </c>
       <c r="F17">
@@ -10131,7 +10897,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5">
-        <f>D21/5</f>
+        <f t="shared" ref="E21:E26" si="4">D21/5</f>
         <v>0</v>
       </c>
     </row>
@@ -10148,11 +10914,11 @@
         <v>10.666666666666666</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:D26" si="2">SUM(B22:C22)</f>
+        <f t="shared" ref="D22:D26" si="5">SUM(B22:C22)</f>
         <v>892.66666666666663</v>
       </c>
       <c r="E22" s="5">
-        <f>D22/5</f>
+        <f t="shared" si="4"/>
         <v>178.53333333333333</v>
       </c>
       <c r="F22">
@@ -10187,11 +10953,11 @@
         <v>18.333333333333332</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1970.6666666666665</v>
       </c>
       <c r="E23" s="5">
-        <f>D23/5</f>
+        <f t="shared" si="4"/>
         <v>394.13333333333333</v>
       </c>
       <c r="F23">
@@ -10226,11 +10992,11 @@
         <v>27</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3096.3333333333335</v>
       </c>
       <c r="E24" s="5">
-        <f>D24/5</f>
+        <f t="shared" si="4"/>
         <v>619.26666666666665</v>
       </c>
       <c r="F24">
@@ -10265,11 +11031,11 @@
         <v>42.333333333333336</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4849.333333333333</v>
       </c>
       <c r="E25" s="5">
-        <f>D25/5</f>
+        <f t="shared" si="4"/>
         <v>969.86666666666656</v>
       </c>
       <c r="F25">
@@ -10304,11 +11070,11 @@
         <v>43.333333333333336</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6418.333333333333</v>
       </c>
       <c r="E26" s="5">
-        <f>D26/5</f>
+        <f t="shared" si="4"/>
         <v>1283.6666666666665</v>
       </c>
       <c r="F26">
@@ -10386,11 +11152,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" ref="D30:D35" si="3">SUM(B30:C30)</f>
+        <f t="shared" ref="D30:D35" si="6">SUM(B30:C30)</f>
         <v>0</v>
       </c>
       <c r="E30" s="5">
-        <f>D30/5</f>
+        <f t="shared" ref="E30:E35" si="7">D30/5</f>
         <v>0</v>
       </c>
     </row>
@@ -10407,11 +11173,11 @@
         <v>207</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>294</v>
       </c>
       <c r="E31" s="5">
-        <f>D31/5</f>
+        <f t="shared" si="7"/>
         <v>58.8</v>
       </c>
       <c r="F31">
@@ -10446,11 +11212,11 @@
         <v>319</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>436.66666666666669</v>
       </c>
       <c r="E32" s="5">
-        <f>D32/5</f>
+        <f t="shared" si="7"/>
         <v>87.333333333333343</v>
       </c>
       <c r="F32">
@@ -10485,11 +11251,11 @@
         <v>494.66666666666669</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>656.33333333333337</v>
       </c>
       <c r="E33" s="5">
-        <f>D33/5</f>
+        <f t="shared" si="7"/>
         <v>131.26666666666668</v>
       </c>
       <c r="F33">
@@ -10524,11 +11290,11 @@
         <v>648.33333333333337</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>840.33333333333337</v>
       </c>
       <c r="E34" s="5">
-        <f>D34/5</f>
+        <f t="shared" si="7"/>
         <v>168.06666666666666</v>
       </c>
       <c r="F34">
@@ -10563,11 +11329,11 @@
         <v>831.33333333333337</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1061</v>
       </c>
       <c r="E35" s="5">
-        <f>D35/5</f>
+        <f t="shared" si="7"/>
         <v>212.2</v>
       </c>
       <c r="F35">
@@ -10646,11 +11412,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" ref="D39:D44" si="4">SUM(B39:C39)</f>
+        <f t="shared" ref="D39:D44" si="8">SUM(B39:C39)</f>
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <f>D39/5</f>
+        <f t="shared" ref="E39:E44" si="9">D39/5</f>
         <v>0</v>
       </c>
     </row>
@@ -10667,11 +11433,11 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>410</v>
       </c>
       <c r="E40" s="5">
-        <f>D40/5</f>
+        <f t="shared" si="9"/>
         <v>82</v>
       </c>
       <c r="F40">
@@ -10706,11 +11472,11 @@
         <v>3</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>801</v>
       </c>
       <c r="E41" s="5">
-        <f>D41/5</f>
+        <f t="shared" si="9"/>
         <v>160.19999999999999</v>
       </c>
       <c r="F41">
@@ -10745,11 +11511,11 @@
         <v>3</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1077.6666666666667</v>
       </c>
       <c r="E42" s="5">
-        <f>D42/5</f>
+        <f t="shared" si="9"/>
         <v>215.53333333333336</v>
       </c>
       <c r="F42">
@@ -10784,11 +11550,11 @@
         <v>3</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1448.6666666666667</v>
       </c>
       <c r="E43" s="5">
-        <f>D43/5</f>
+        <f t="shared" si="9"/>
         <v>289.73333333333335</v>
       </c>
       <c r="F43">
@@ -10823,11 +11589,11 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1817.3333333333333</v>
       </c>
       <c r="E44" s="5">
-        <f>D44/5</f>
+        <f t="shared" si="9"/>
         <v>363.46666666666664</v>
       </c>
       <c r="F44">
@@ -10906,11 +11672,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" ref="D48:D53" si="5">SUM(B48:C48)</f>
+        <f t="shared" ref="D48:D53" si="10">SUM(B48:C48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <f>D48/5</f>
+        <f t="shared" ref="E48:E53" si="11">D48/5</f>
         <v>0</v>
       </c>
     </row>
@@ -10927,11 +11693,11 @@
         <v>24.666666666666668</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>262.33333333333331</v>
       </c>
       <c r="E49" s="5">
-        <f>D49/5</f>
+        <f t="shared" si="11"/>
         <v>52.466666666666661</v>
       </c>
       <c r="F49">
@@ -10966,11 +11732,11 @@
         <v>43</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>379</v>
       </c>
       <c r="E50" s="5">
-        <f>D50/5</f>
+        <f t="shared" si="11"/>
         <v>75.8</v>
       </c>
       <c r="F50">
@@ -11005,11 +11771,11 @@
         <v>64.666666666666671</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>549.66666666666663</v>
       </c>
       <c r="E51" s="5">
-        <f>D51/5</f>
+        <f t="shared" si="11"/>
         <v>109.93333333333332</v>
       </c>
       <c r="F51">
@@ -11044,11 +11810,11 @@
         <v>88</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>660</v>
       </c>
       <c r="E52" s="5">
-        <f>D52/5</f>
+        <f t="shared" si="11"/>
         <v>132</v>
       </c>
       <c r="F52">
@@ -11083,11 +11849,11 @@
         <v>100.66666666666667</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>862.66666666666663</v>
       </c>
       <c r="E53" s="5">
-        <f>D53/5</f>
+        <f t="shared" si="11"/>
         <v>172.53333333333333</v>
       </c>
       <c r="F53">
@@ -11112,6 +11878,236 @@
     <row r="54" spans="1:11" s="2" customFormat="1" ht="150" customHeight="1">
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
+    </row>
+    <row r="70" spans="1:11" s="1" customFormat="1">
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" t="s">
+        <v>9</v>
+      </c>
+      <c r="K71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <f>SUM(B72:C72)</f>
+        <v>0</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" ref="E72:E77" si="12">D72/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <f>AVERAGE(F73:H73)</f>
+        <v>787.5</v>
+      </c>
+      <c r="C73">
+        <f>AVERAGE(I73:K73)</f>
+        <v>8.5</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" ref="D73:D77" si="13">SUM(B73:C73)</f>
+        <v>796</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="12"/>
+        <v>159.19999999999999</v>
+      </c>
+      <c r="F73">
+        <v>793</v>
+      </c>
+      <c r="G73">
+        <v>782</v>
+      </c>
+      <c r="I73">
+        <v>8</v>
+      </c>
+      <c r="J73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <f>AVERAGE(F74:H74)</f>
+        <v>1524.5</v>
+      </c>
+      <c r="C74">
+        <f>AVERAGE(I74:K74)</f>
+        <v>14</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="13"/>
+        <v>1538.5</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="12"/>
+        <v>307.7</v>
+      </c>
+      <c r="F74">
+        <v>1521</v>
+      </c>
+      <c r="G74">
+        <v>1528</v>
+      </c>
+      <c r="I74">
+        <v>14</v>
+      </c>
+      <c r="J74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>60</v>
+      </c>
+      <c r="B75">
+        <f>AVERAGE(F75:H75)</f>
+        <v>2628</v>
+      </c>
+      <c r="C75">
+        <f>AVERAGE(I75:K75)</f>
+        <v>23.5</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="13"/>
+        <v>2651.5</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="12"/>
+        <v>530.29999999999995</v>
+      </c>
+      <c r="F75">
+        <v>2622</v>
+      </c>
+      <c r="G75">
+        <v>2634</v>
+      </c>
+      <c r="I75">
+        <v>24</v>
+      </c>
+      <c r="J75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <f>AVERAGE(F76:H76)</f>
+        <v>4029.5</v>
+      </c>
+      <c r="C76">
+        <f>AVERAGE(I76:K76)</f>
+        <v>35.5</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="13"/>
+        <v>4065</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="12"/>
+        <v>813</v>
+      </c>
+      <c r="F76">
+        <v>4261</v>
+      </c>
+      <c r="G76">
+        <v>3798</v>
+      </c>
+      <c r="I76">
+        <v>42</v>
+      </c>
+      <c r="J76">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>100</v>
+      </c>
+      <c r="B77">
+        <f>AVERAGE(F77:H77)</f>
+        <v>5201.5</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(I77:K77)</f>
+        <v>35</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="13"/>
+        <v>5236.5</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="12"/>
+        <v>1047.3</v>
+      </c>
+      <c r="F77">
+        <v>5246</v>
+      </c>
+      <c r="G77">
+        <v>5157</v>
+      </c>
+      <c r="I77">
+        <v>35</v>
+      </c>
+      <c r="J77">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="150" customHeight="1">
+      <c r="D78" s="4"/>
+      <c r="E78" s="6"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>

</xml_diff>